<commit_message>
Refactor HpBar system to NPC-only architecture
Move HpBar widget functionality from base character class to NPC-specific implementation. Player characters now rely on HUD for health display while NPCs retain individual health bars that appear on damage and disappear on death.

Key changes:
- Remove HpBar component from RSCharacterBase
- Add HpBar functionality to RSCharacterNonPlayer with socket fallback
- Update interface implementations for proper widget handling
- Add Stickman character to game data and enums
- Improve attack sound integration and debug visualization
</commit_message>
<xml_diff>
--- a/GameData/RSCharacterStatTable.xlsx
+++ b/GameData/RSCharacterStatTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Project_RS\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF61B23-A649-4205-8FD1-DD45D67F31C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E02980-5459-4DC5-9375-E86E4075AEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9390" yWindow="2960" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9390" yWindow="3140" windowWidth="28800" windowHeight="15190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +56,10 @@
   </si>
   <si>
     <t>Teuthisan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stickman</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -381,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F4"/>
+  <dimension ref="A2:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -453,6 +457,26 @@
         <v>300</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>350</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>